<commit_message>
Add import tickets glpi
</commit_message>
<xml_diff>
--- a/templates/template1.xlsx
+++ b/templates/template1.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4E40BC0-0334-4BD1-B3DF-4DC427DA847C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewProjects\AdvLicenceManager\adv-tickets-backend\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,80 +32,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Pais</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Direccion</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Nombre de contacto</t>
-  </si>
-  <si>
-    <t>Telefono de contacto</t>
-  </si>
-  <si>
-    <t>${table:clients.dni}</t>
-  </si>
-  <si>
-    <t>${table:clients.name}</t>
-  </si>
-  <si>
-    <t>${table:clients.country}</t>
-  </si>
-  <si>
-    <t>${table:clients.trademark}</t>
-  </si>
-  <si>
-    <t>${table:clients.address}</t>
-  </si>
-  <si>
-    <t>${table:clients.phone}</t>
-  </si>
-  <si>
-    <t>${table:clients.email}</t>
-  </si>
-  <si>
-    <t>${table:clients.contactName}</t>
-  </si>
-  <si>
-    <t>${table:clients.contactPhone}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>${table:tickets.id}</t>
+  </si>
+  <si>
+    <t>glpi_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>closedate</t>
+  </si>
+  <si>
+    <t>solvedate</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>urgency</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>date_creation</t>
+  </si>
+  <si>
+    <t>${table:tickets.title}</t>
+  </si>
+  <si>
+    <t>${table:tickets.date}</t>
+  </si>
+  <si>
+    <t>${table:tickets.closedate}</t>
+  </si>
+  <si>
+    <t>${table:tickets.solvedate}</t>
+  </si>
+  <si>
+    <t>${table:tickets.status}</t>
+  </si>
+  <si>
+    <t>${table:tickets.description}</t>
+  </si>
+  <si>
+    <t>${table:tickets.urgency}</t>
+  </si>
+  <si>
+    <t>${table:tickets.impact}</t>
+  </si>
+  <si>
+    <t>${table:tickets.priority}</t>
+  </si>
+  <si>
+    <t>${table:tickets.type}</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>${table:tickets.userGlpiId}</t>
+  </si>
+  <si>
+    <t>${table:tickets.dateCreation}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,9 +145,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,18 +460,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -477,37 +497,62 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" t="s">
         <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>